<commit_message>
improve bibliography and string handling
Switched package stringi to stringr to simplify string handling (needs a little more code clean-up). Added tab-separated table of possible citations. Expanded spreadsheet examples. Edited code to conditionally apply citations (work in progress).
</commit_message>
<xml_diff>
--- a/metadata_inputs.xlsx
+++ b/metadata_inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Michelle\Code\R_code\SimplifiedMetadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Michelle\Metadata\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Inputs</t>
   </si>
@@ -98,13 +98,49 @@
     <t>Code2</t>
   </si>
   <si>
+    <t>Oceanodroma melania</t>
+  </si>
+  <si>
+    <t>Black Storm-Petrel</t>
+  </si>
+  <si>
+    <t>oceamela_AltMap_20190228.tif</t>
+  </si>
+  <si>
+    <t>Element Occurrences (EOs)</t>
+  </si>
+  <si>
+    <t>Agathymus gentryi</t>
+  </si>
+  <si>
+    <t>Gentry's Giant-Skipper</t>
+  </si>
+  <si>
     <t>oceahomo</t>
   </si>
   <si>
-    <t>Element Occurrences (EOs)</t>
-  </si>
-  <si>
-    <t>1 km grid cells containing the breeding EOs were used as the model</t>
+    <t>oceamela</t>
+  </si>
+  <si>
+    <t>agatgent_AltMap_20190417.tif</t>
+  </si>
+  <si>
+    <t>agatgent</t>
+  </si>
+  <si>
+    <t>Arizona Heritage Data Management System</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>Element Occurrences (EOs), Butterflies and Moths of North America (BAMONA), Land Cover, and Elevation</t>
+  </si>
+  <si>
+    <t>created using EOs plus BAMONA locations to inform land cover (pinyon-juniper and desert scrub) and topography (intermediately to moderately rugged) selections</t>
+  </si>
+  <si>
+    <t>a simple selection of 1 km grid cells containing the breeding EOs</t>
   </si>
 </sst>
 </file>
@@ -659,14 +695,14 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.28515625" bestFit="1" customWidth="1"/>
@@ -675,7 +711,7 @@
     <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="68.42578125" customWidth="1"/>
     <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -731,7 +767,7 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>102988</v>
@@ -740,7 +776,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
         <v>21</v>
@@ -758,12 +794,100 @@
         <v>8</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="M2" t="s">
         <v>17</v>
       </c>
       <c r="N2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>105368</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4">
+        <v>116354</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -812,9 +936,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId2"/>
+    <hyperlink ref="K4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>